<commit_message>
Ajustement de quelque fonction
Fonction .csv pour ajouter des donnés simplifié.
Ajout de la liste de chose à fair pour finir la toure.
</commit_message>
<xml_diff>
--- a/Fiber_Drawing_Tower/Concept_GUI.xlsx
+++ b/Fiber_Drawing_Tower/Concept_GUI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephgaulin/Documents/GitHub/nanocomposite-fab/Fiber_Drawing_Tower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A436393-A12A-B249-8CF3-1747B26D0C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6637ACD-F9D2-0B47-875B-FE57E8255574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{7F0DE0F7-3FA3-ED4B-9728-61F0AEEDDAE6}"/>
+    <workbookView xWindow="1200" yWindow="1880" windowWidth="28040" windowHeight="17440" xr2:uid="{7F0DE0F7-3FA3-ED4B-9728-61F0AEEDDAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Diamètre</t>
-  </si>
-  <si>
-    <t>Longueur</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Graphique</t>
   </si>
@@ -55,13 +49,34 @@
     <t>Ajuster l'échelle</t>
   </si>
   <si>
-    <t>Vitesse</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
     <t>Apply</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Speed of motor</t>
+  </si>
+  <si>
+    <t>Name of the file</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -123,19 +138,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,15 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F747C227-C423-8249-8A59-B61BBBC28BE0}">
-  <dimension ref="D5:M27"/>
+  <dimension ref="D5:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -470,8 +485,9 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -482,92 +498,106 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="K7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="J9" s="1"/>
+      <c r="K9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="I11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -575,11 +605,16 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="K13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -590,8 +625,9 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -602,8 +638,9 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -614,108 +651,117 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="1"/>
+      <c r="E17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="1"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="1"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="1"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="1"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="1"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -726,22 +772,24 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
-      <c r="E26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="1"/>
+      <c r="E26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -752,12 +800,13 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="E17:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>